<commit_message>
Update app constants and refactor baseExportService
</commit_message>
<xml_diff>
--- a/src/main/resources/static/templates/excel/Template_E_Product.xlsx
+++ b/src/main/resources/static/templates/excel/Template_E_Product.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App\FW_PMS\src\main\resources\static\templates\excel\"/>
     </mc:Choice>
@@ -70,6 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -557,7 +558,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
@@ -565,15 +566,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" style="1" customWidth="1"/>
-    <col min="4" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19" style="1" customWidth="1"/>
-    <col min="12" max="1025" width="8.85546875" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="4.5703125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="16.7109375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="41.140625" collapsed="false"/>
+    <col min="4" max="6" customWidth="true" style="1" width="12.7109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="1" width="15.42578125" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="16.140625" collapsed="false"/>
+    <col min="9" max="10" customWidth="true" style="1" width="10.28515625" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="1" width="19.0" collapsed="false"/>
+    <col min="12" max="1025" style="1" width="8.85546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>